<commit_message>
Actualizar instrucciones de instalación en README.MD
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daviidco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\whatsapp-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DA400F-5B15-4FB4-B7DE-E5DE9870FCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD52F08-6600-4A6C-82A5-62FC057F95BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3048" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{0C66EDC1-370A-4BC8-8510-9CFEC6A2C674}"/>
+    <workbookView xWindow="3630" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{0C66EDC1-370A-4BC8-8510-9CFEC6A2C674}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>numero</t>
   </si>
@@ -39,27 +39,47 @@
     <t>años</t>
   </si>
   <si>
-    <t>david</t>
-  </si>
-  <si>
-    <t>mariluz</t>
-  </si>
-  <si>
-    <t>Pauli</t>
-  </si>
-  <si>
-    <t>mariluz 3</t>
-  </si>
-  <si>
-    <t>+573178999999</t>
+    <t>+51986687645</t>
+  </si>
+  <si>
+    <t>+51948345071</t>
+  </si>
+  <si>
+    <t>+51976216498</t>
+  </si>
+  <si>
+    <t>Jhonny Romero</t>
+  </si>
+  <si>
+    <t>Laredo 666</t>
+  </si>
+  <si>
+    <t>Luis Cachay</t>
+  </si>
+  <si>
+    <t>El bosque caperucita</t>
+  </si>
+  <si>
+    <t>Enrique Incio</t>
+  </si>
+  <si>
+    <t>BR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,9 +107,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,19 +425,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82880A35-97B6-477A-8E2C-92E9B83FAB0D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -429,32 +452,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D4" s="2">
         <v>7</v>
-      </c>
-      <c r="D3">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>